<commit_message>
Add TOC4 to pages validation
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_workbook.xlsx
+++ b/openn/tests/data/sheets/valid_workbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4467" uniqueCount="3974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="3976">
   <si>
     <t>1r</t>
   </si>
@@ -11981,6 +11981,12 @@
   </si>
   <si>
     <t>Smith, John (1843-1909)</t>
+  </si>
+  <si>
+    <t>TOC4</t>
+  </si>
+  <si>
+    <t>Octobe 3, 1904</t>
   </si>
 </sst>
 </file>
@@ -12551,7 +12557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -13667,9 +13673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B102" sqref="B102:B1403"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14031,7 +14037,7 @@
         <v>3708</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:12">
       <c r="B17" s="3">
         <v>14</v>
       </c>
@@ -14059,8 +14065,14 @@
       <c r="J17" s="15" t="s">
         <v>3711</v>
       </c>
-    </row>
-    <row r="18" spans="2:10">
+      <c r="K17" s="2" t="s">
+        <v>3974</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="3">
         <v>15</v>
       </c>
@@ -14083,7 +14095,7 @@
         <v>3713</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:12">
       <c r="B19" s="3">
         <v>16</v>
       </c>
@@ -14106,7 +14118,7 @@
         <v>3715</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:12">
       <c r="B20" s="3">
         <v>17</v>
       </c>
@@ -14129,7 +14141,7 @@
         <v>3717</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:12">
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -14152,7 +14164,7 @@
         <v>3719</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:12">
       <c r="B22" s="3">
         <v>19</v>
       </c>
@@ -14175,7 +14187,7 @@
         <v>3721</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:12">
       <c r="B23" s="3">
         <v>20</v>
       </c>
@@ -14204,7 +14216,7 @@
         <v>3724</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:12">
       <c r="B24" s="3">
         <v>21</v>
       </c>
@@ -14221,7 +14233,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:12">
       <c r="B25" s="3">
         <v>22</v>
       </c>
@@ -14244,7 +14256,7 @@
         <v>3727</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:12">
       <c r="B26" s="3">
         <v>23</v>
       </c>
@@ -14267,7 +14279,7 @@
         <v>3729</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:12">
       <c r="B27" s="3">
         <v>24</v>
       </c>
@@ -14290,7 +14302,7 @@
         <v>3731</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:12">
       <c r="B28" s="3">
         <v>25</v>
       </c>
@@ -14313,7 +14325,7 @@
         <v>3733</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:12">
       <c r="B29" s="3">
         <v>26</v>
       </c>
@@ -14336,7 +14348,7 @@
         <v>3735</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:12">
       <c r="B30" s="3">
         <v>27</v>
       </c>
@@ -14359,7 +14371,7 @@
         <v>3737</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:12">
       <c r="B31" s="3">
         <v>28</v>
       </c>
@@ -14382,7 +14394,7 @@
         <v>3739</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:12">
       <c r="B32" s="3">
         <v>29</v>
       </c>
@@ -16100,36 +16112,72 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'VALUE LISTS'!$B$3:$B$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>E5:E1403</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
-          <x14:formula1>
-            <xm:f>'VALUE LISTS'!$B$3:$B$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3 K1405</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select the page counting method" prompt="[required]_x000d__x000d_Options: Foliation, Pagination_x000d__x000d_Choose the primary method used for enumerating the pages in this diary.">
           <x14:formula1>
             <xm:f>'VALUE LISTS'!$F$3:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>B1</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5:E1403</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>K1405</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
           <x14:formula1>
-            <xm:f>'VALUE LISTS'!$B$3:$B$10</xm:f>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>I5:I1404 G5:G1403 K5:K1404</xm:sqref>
+          <xm:sqref>I5:I1404</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5:G1403</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_FIG -- any other type of figure">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>K5:K1404</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2, TOC3 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_BLANK -- the page or folio side is blank (no value required)">
           <x14:formula1>
-            <xm:f>'VALUE LISTS'!$B$3:$B$10</xm:f>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>G4 I4 K4 E4</xm:sqref>
+          <xm:sqref>G4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2, TOC3 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_BLANK -- the page or folio side is blank (no value required)">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>I4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2, TOC3 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_BLANK -- the page or folio side is blank (no value required)">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tag" prompt="[optional]_x000d__x000d_The type for an extra label of this image. Examples:_x000d__x000d_TOC1, TOC2, TOC3 -- table of contents entries_x000d_ILL -- illumination or pictoral illustraion_x000d_BLANK -- the page or folio side is blank (no value required)">
+          <x14:formula1>
+            <xm:f>'VALUE LISTS'!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -33563,10 +33611,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -33614,11 +33662,16 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>2620</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
         <v>3667</v>
       </c>
     </row>

</xml_diff>